<commit_message>
Added Feature to extract .msg attatchments
</commit_message>
<xml_diff>
--- a/Combined Form Data.xlsx
+++ b/Combined Form Data.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="87">
   <si>
     <t>Recently Married</t>
   </si>
@@ -262,16 +262,19 @@
     <t>totalPoints</t>
   </si>
   <si>
-    <t>2021/08/13</t>
-  </si>
-  <si>
-    <t>Completed</t>
-  </si>
-  <si>
-    <t>Josh</t>
-  </si>
-  <si>
-    <t>Agency</t>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>2022/01/08</t>
+  </si>
+  <si>
+    <t>Chris Gryzen</t>
+  </si>
+  <si>
+    <t>Josh Gryzen</t>
+  </si>
+  <si>
+    <t>Gryzen</t>
   </si>
 </sst>
 </file>
@@ -629,7 +632,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:CD2"/>
+  <dimension ref="A1:CD5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -884,17 +887,167 @@
       </c>
     </row>
     <row r="2" spans="1:82">
+      <c r="N2" t="s">
+        <v>82</v>
+      </c>
+      <c r="R2" t="s">
+        <v>82</v>
+      </c>
+      <c r="W2" t="s">
+        <v>82</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>82</v>
+      </c>
       <c r="AI2" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="AJ2" t="s">
+        <v>84</v>
+      </c>
+      <c r="AK2" t="s">
+        <v>85</v>
+      </c>
+      <c r="AL2" t="s">
+        <v>86</v>
+      </c>
+      <c r="AQ2" t="s">
+        <v>82</v>
+      </c>
+      <c r="BN2" t="s">
+        <v>82</v>
+      </c>
+      <c r="BU2" t="s">
+        <v>82</v>
+      </c>
+      <c r="BW2" t="s">
+        <v>82</v>
+      </c>
+      <c r="CD2">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:82">
+      <c r="N3" t="s">
+        <v>82</v>
+      </c>
+      <c r="R3" t="s">
+        <v>82</v>
+      </c>
+      <c r="W3" t="s">
+        <v>82</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>82</v>
+      </c>
+      <c r="AI3" t="s">
         <v>83</v>
       </c>
-      <c r="AK2" t="s">
+      <c r="AJ3" t="s">
         <v>84</v>
       </c>
-      <c r="AL2" t="s">
+      <c r="AK3" t="s">
         <v>85</v>
+      </c>
+      <c r="AL3" t="s">
+        <v>86</v>
+      </c>
+      <c r="AQ3" t="s">
+        <v>82</v>
+      </c>
+      <c r="BN3" t="s">
+        <v>82</v>
+      </c>
+      <c r="BU3" t="s">
+        <v>82</v>
+      </c>
+      <c r="BW3" t="s">
+        <v>82</v>
+      </c>
+      <c r="CD3">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:82">
+      <c r="N4" t="s">
+        <v>82</v>
+      </c>
+      <c r="R4" t="s">
+        <v>82</v>
+      </c>
+      <c r="W4" t="s">
+        <v>82</v>
+      </c>
+      <c r="Y4" t="s">
+        <v>82</v>
+      </c>
+      <c r="AI4" t="s">
+        <v>83</v>
+      </c>
+      <c r="AJ4" t="s">
+        <v>84</v>
+      </c>
+      <c r="AK4" t="s">
+        <v>85</v>
+      </c>
+      <c r="AL4" t="s">
+        <v>86</v>
+      </c>
+      <c r="AQ4" t="s">
+        <v>82</v>
+      </c>
+      <c r="BN4" t="s">
+        <v>82</v>
+      </c>
+      <c r="BU4" t="s">
+        <v>82</v>
+      </c>
+      <c r="BW4" t="s">
+        <v>82</v>
+      </c>
+      <c r="CD4">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:82">
+      <c r="N5" t="s">
+        <v>82</v>
+      </c>
+      <c r="R5" t="s">
+        <v>82</v>
+      </c>
+      <c r="W5" t="s">
+        <v>82</v>
+      </c>
+      <c r="Y5" t="s">
+        <v>82</v>
+      </c>
+      <c r="AI5" t="s">
+        <v>83</v>
+      </c>
+      <c r="AJ5" t="s">
+        <v>84</v>
+      </c>
+      <c r="AK5" t="s">
+        <v>85</v>
+      </c>
+      <c r="AL5" t="s">
+        <v>86</v>
+      </c>
+      <c r="AQ5" t="s">
+        <v>82</v>
+      </c>
+      <c r="BN5" t="s">
+        <v>82</v>
+      </c>
+      <c r="BU5" t="s">
+        <v>82</v>
+      </c>
+      <c r="BW5" t="s">
+        <v>82</v>
+      </c>
+      <c r="CD5">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Cleaned up a bit
</commit_message>
<xml_diff>
--- a/Combined Form Data.xlsx
+++ b/Combined Form Data.xlsx
@@ -1,20 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24729"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cjgry\Documents\Python Excel Executable\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3CF41E2-6131-42C4-814D-BA3DF6C03EBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="82">
   <si>
     <t>Recently Married</t>
   </si>
@@ -260,28 +266,13 @@
   </si>
   <si>
     <t>totalPoints</t>
-  </si>
-  <si>
-    <t>Yes</t>
-  </si>
-  <si>
-    <t>2022/01/08</t>
-  </si>
-  <si>
-    <t>Chris Gryzen</t>
-  </si>
-  <si>
-    <t>Josh Gryzen</t>
-  </si>
-  <si>
-    <t>Gryzen</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -344,6 +335,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -390,7 +389,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -422,9 +421,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -456,6 +473,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -631,14 +666,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:CD5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:CD1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD5"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:82">
+    <row r="1" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -884,170 +921,6 @@
       </c>
       <c r="CD1" s="1" t="s">
         <v>81</v>
-      </c>
-    </row>
-    <row r="2" spans="1:82">
-      <c r="N2" t="s">
-        <v>82</v>
-      </c>
-      <c r="R2" t="s">
-        <v>82</v>
-      </c>
-      <c r="W2" t="s">
-        <v>82</v>
-      </c>
-      <c r="Y2" t="s">
-        <v>82</v>
-      </c>
-      <c r="AI2" t="s">
-        <v>83</v>
-      </c>
-      <c r="AJ2" t="s">
-        <v>84</v>
-      </c>
-      <c r="AK2" t="s">
-        <v>85</v>
-      </c>
-      <c r="AL2" t="s">
-        <v>86</v>
-      </c>
-      <c r="AQ2" t="s">
-        <v>82</v>
-      </c>
-      <c r="BN2" t="s">
-        <v>82</v>
-      </c>
-      <c r="BU2" t="s">
-        <v>82</v>
-      </c>
-      <c r="BW2" t="s">
-        <v>82</v>
-      </c>
-      <c r="CD2">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="3" spans="1:82">
-      <c r="N3" t="s">
-        <v>82</v>
-      </c>
-      <c r="R3" t="s">
-        <v>82</v>
-      </c>
-      <c r="W3" t="s">
-        <v>82</v>
-      </c>
-      <c r="Y3" t="s">
-        <v>82</v>
-      </c>
-      <c r="AI3" t="s">
-        <v>83</v>
-      </c>
-      <c r="AJ3" t="s">
-        <v>84</v>
-      </c>
-      <c r="AK3" t="s">
-        <v>85</v>
-      </c>
-      <c r="AL3" t="s">
-        <v>86</v>
-      </c>
-      <c r="AQ3" t="s">
-        <v>82</v>
-      </c>
-      <c r="BN3" t="s">
-        <v>82</v>
-      </c>
-      <c r="BU3" t="s">
-        <v>82</v>
-      </c>
-      <c r="BW3" t="s">
-        <v>82</v>
-      </c>
-      <c r="CD3">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:82">
-      <c r="N4" t="s">
-        <v>82</v>
-      </c>
-      <c r="R4" t="s">
-        <v>82</v>
-      </c>
-      <c r="W4" t="s">
-        <v>82</v>
-      </c>
-      <c r="Y4" t="s">
-        <v>82</v>
-      </c>
-      <c r="AI4" t="s">
-        <v>83</v>
-      </c>
-      <c r="AJ4" t="s">
-        <v>84</v>
-      </c>
-      <c r="AK4" t="s">
-        <v>85</v>
-      </c>
-      <c r="AL4" t="s">
-        <v>86</v>
-      </c>
-      <c r="AQ4" t="s">
-        <v>82</v>
-      </c>
-      <c r="BN4" t="s">
-        <v>82</v>
-      </c>
-      <c r="BU4" t="s">
-        <v>82</v>
-      </c>
-      <c r="BW4" t="s">
-        <v>82</v>
-      </c>
-      <c r="CD4">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5" spans="1:82">
-      <c r="N5" t="s">
-        <v>82</v>
-      </c>
-      <c r="R5" t="s">
-        <v>82</v>
-      </c>
-      <c r="W5" t="s">
-        <v>82</v>
-      </c>
-      <c r="Y5" t="s">
-        <v>82</v>
-      </c>
-      <c r="AI5" t="s">
-        <v>83</v>
-      </c>
-      <c r="AJ5" t="s">
-        <v>84</v>
-      </c>
-      <c r="AK5" t="s">
-        <v>85</v>
-      </c>
-      <c r="AL5" t="s">
-        <v>86</v>
-      </c>
-      <c r="AQ5" t="s">
-        <v>82</v>
-      </c>
-      <c r="BN5" t="s">
-        <v>82</v>
-      </c>
-      <c r="BU5" t="s">
-        <v>82</v>
-      </c>
-      <c r="BW5" t="s">
-        <v>82</v>
-      </c>
-      <c r="CD5">
-        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>